<commit_message>
Revert "Testing binary changes"
This reverts commit 1d48987143302bab37c65e28a10825443fc399c5.
</commit_message>
<xml_diff>
--- a/BMS/MasterData.xlsx
+++ b/BMS/MasterData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>ServiceKey</t>
   </si>
@@ -97,9 +97,6 @@
   </si>
   <si>
     <t>PHNhbWw6QXNzZXJ0aW9uIE1ham9yVmVyc2lvbj0iMSIgTWlub3JWZXJzaW9uPSIxIiBBc3NlcnRpb25JRD0iXzgyYTE5ZTlkLTI2ZmQtNDhlOC05MzRlLTc4OGYxMzE3YTZhMyIgSXNzdWVyPSJJcGNBdXRoZW50aWNhdGlvbiIgSXNzdWVJbnN0YW50PSIyMDExLTAyLTI0VDE4OjEzOjQ4LjI2N1oiIHhtbG5zOnNhbWw9InVybjpvYXNpczpuYW1lczp0YzpTQU1MOjEuMDphc3NlcnRpb24iPjxzYW1sOkNvbmRpdGlvbnMgTm90QmVmb3JlPSIyMDExLTAyLTI0VDE4OjEzOjQ4LjI2N1oiIE5vdE9uT3JBZnRlcj0iMjAxNC0wMi0yNFQxODoxMzo0OC4yNjdaIj48L3NhbWw6Q29uZGl0aW9ucz48c2FtbDpBZHZpY2U+PC9zYW1sOkFkdmljZT48c2FtbDpBdHRyaWJ1dGVTdGF0ZW1lbnQ+PHNhbWw6U3ViamVjdD48c2FtbDpOYW1lSWRlbnRpZmllcj5CRUVCQjU3NEEyMDAwMDExPC9zYW1sOk5hbWVJZGVudGlmaWVyPjwvc2FtbDpTdWJqZWN0PjxzYW1sOkF0dHJpYnV0ZSBBdHRyaWJ1dGVOYW1lPSJTQUsiIEF0dHJpYnV0ZU5hbWVzcGFjZT0iaHR0cDovL3NjaGVtYXMuaXBjb21tZXJjZS5jb20vSWRlbnRpdHkiPjxzYW1sOkF0dHJpYnV0ZVZhbHVlPkJFRUJCNTc0QTIwMDAwMTE8L3NhbWw6QXR0cmlidXRlVmFsdWU+PC9zYW1sOkF0dHJpYnV0ZT48c2FtbDpBdHRyaWJ1dGUgQXR0cmlidXRlTmFtZT0iU2VyaWFsIiBBdHRyaWJ1dGVOYW1lc3BhY2U9Imh0dHA6Ly9zY2hlbWFzLmlwY29tbWVyY2UuY29tL0lkZW50aXR5Ij48c2FtbDpBdHRyaWJ1dGVWYWx1ZT4xZDg4YWUzYy0zNzQwLTQzMWEtOTA1Ny0zNTkxMDc4ODJiMDQ8L3NhbWw6QXR0cmlidXRlVmFsdWU+PC9zYW1sOkF0dHJpYnV0ZT48c2FtbDpBdHRyaWJ1dGUgQXR0cmlidXRlTmFtZT0ibmFtZSIgQXR0cmlidXRlTmFtZXNwYWNlPSJodHRwOi8vc2NoZW1hcy54bWxzb2FwLm9yZy93cy8yMDA1LzA1L2lkZW50aXR5L2NsYWltcyI+PHNhbWw6QXR0cmlidXRlVmFsdWU+QkVFQkI1NzRBMjAwMDAxMTwvc2FtbDpBdHRyaWJ1dGVWYWx1ZT48L3NhbWw6QXR0cmlidXRlPjwvc2FtbDpBdHRyaWJ1dGVTdGF0ZW1lbnQ+PFNpZ25hdHVyZSB4bWxucz0iaHR0cDovL3d3dy53My5vcmcvMjAwMC8wOS94bWxkc2lnIyI+PFNpZ25lZEluZm8+PENhbm9uaWNhbGl6YXRpb25NZXRob2QgQWxnb3JpdGhtPSJodHRwOi8vd3d3LnczLm9yZy8yMDAxLzEwL3htbC1leGMtYzE0biMiPjwvQ2Fub25pY2FsaXphdGlvbk1ldGhvZD48U2lnbmF0dXJlTWV0aG9kIEFsZ29yaXRobT0iaHR0cDovL3d3dy53My5vcmcvMjAwMC8wOS94bWxkc2lnI3JzYS1zaGExIj48L1NpZ25hdHVyZU1ldGhvZD48UmVmZXJlbmNlIFVSST0iI184MmExOWU5ZC0yNmZkLTQ4ZTgtOTM0ZS03ODhmMTMxN2E2YTMiPjxUcmFuc2Zvcm1zPjxUcmFuc2Zvcm0gQWxnb3JpdGhtPSJodHRwOi8vd3d3LnczLm9yZy8yMDAwLzA5L3htbGRzaWcjZW52ZWxvcGVkLXNpZ25hdHVyZSI+PC9UcmFuc2Zvcm0+PFRyYW5zZm9ybSBBbGdvcml0aG09Imh0dHA6Ly93d3cudzMub3JnLzIwMDEvMTAveG1sLWV4Yy1jMTRuIyI+PC9UcmFuc2Zvcm0+PC9UcmFuc2Zvcm1zPjxEaWdlc3RNZXRob2QgQWxnb3JpdGhtPSJodHRwOi8vd3d3LnczLm9yZy8yMDAwLzA5L3htbGRzaWcjc2hhMSI+PC9EaWdlc3RNZXRob2Q+PERpZ2VzdFZhbHVlPm96VWNpb3YwSGVLNERUVmRvclBWN1NodDlwWT08L0RpZ2VzdFZhbHVlPjwvUmVmZXJlbmNlPjwvU2lnbmVkSW5mbz48U2lnbmF0dXJlVmFsdWU+SFlIY3pXTCtQRmNWTlBpYWhEeEdFeXVtNnppODFpZkJsNHpycG5yR2VJeko2Y2NSdXAyWHNXUlgxN1NMQ3JjSU9BVnpXeDRnMUw3NDVQOThDVkVpOFJyc3RQVHlJVURqbzRJQlowQThtM2F0akxQcDVyeVlCbFFTR0E2eUMvY2VXeXJvT095eVB1MW80UERYcjkxNjBHaE9XWXJ2MWl4NWNjZFlnZHpQMCthYnZwT1VaUTlJbkNnZ1ZQUk1YWDllSjFndnZEcTQwWUZHS2NuVmM0V2dQTURsVk1LSEluMlhxRncvZHF3VDZkQWwvRGdGUVRmTzBacHJSc1gwT013WGFDMkNibm04UXMvRGFIMFRPM0ttcU8wVzU1STNhY2R3YS9yallWMmUzeFpDbnU2NjE2emtTWmViV2RXSWJrS0pmNXlvRFlRZ0ZGVDh0MS9hZml5MXdnPT08L1NpZ25hdHVyZVZhbHVlPjxLZXlJbmZvPjxvOlNlY3VyaXR5VG9rZW5SZWZlcmVuY2UgeG1sbnM6bz0iaHR0cDovL2RvY3Mub2FzaXMtb3Blbi5vcmcvd3NzLzIwMDQvMDEvb2FzaXMtMjAwNDAxLXdzcy13c3NlY3VyaXR5LXNlY2V4dC0xLjAueHNkIj48bzpLZXlJZGVudGlmaWVyIFZhbHVlVHlwZT0iaHR0cDovL2RvY3Mub2FzaXMtb3Blbi5vcmcvd3NzL29hc2lzLXdzcy1zb2FwLW1lc3NhZ2Utc2VjdXJpdHktMS4xI1RodW1icHJpbnRTSEExIj50V25KWDk4LzJIamhKMEdlV3R6Y2hSeCs1Ymc9PC9vOktleUlkZW50aWZpZXI+PC9vOlNlY3VyaXR5VG9rZW5SZWZlcmVuY2U+PC9LZXlJbmZvPjwvU2lnbmF0dXJlPjwvc2FtbDpBc3NlcnRpb24+</t>
-  </si>
-  <si>
-    <t>test</t>
   </si>
 </sst>
 </file>
@@ -450,10 +447,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -522,11 +519,6 @@
       </c>
       <c r="F3" s="1" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>